<commit_message>
visualizing overlap + geocode differences
</commit_message>
<xml_diff>
--- a/acs/all_elections_with_tracts.xlsx
+++ b/acs/all_elections_with_tracts.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19741,11 +19741,7 @@
       <c r="G434" t="n">
         <v>2021</v>
       </c>
-      <c r="H434" t="inlineStr">
-        <is>
-          <t>san_francisco_city_council_2012.csv</t>
-        </is>
-      </c>
+      <c r="H434" t="inlineStr"/>
       <c r="I434" t="inlineStr"/>
       <c r="J434" t="inlineStr"/>
     </row>
@@ -19829,11 +19825,7 @@
       <c r="G436" t="n">
         <v>2021</v>
       </c>
-      <c r="H436" t="inlineStr">
-        <is>
-          <t>san_francisco_city_council_2012.csv</t>
-        </is>
-      </c>
+      <c r="H436" t="inlineStr"/>
       <c r="I436" t="inlineStr"/>
       <c r="J436" t="inlineStr"/>
     </row>
@@ -20015,11 +20007,19 @@
       </c>
       <c r="H440" t="inlineStr">
         <is>
-          <t>san_francisco_city_council_2022.csv</t>
-        </is>
-      </c>
-      <c r="I440" t="inlineStr"/>
-      <c r="J440" t="inlineStr"/>
+          <t>takoma_park_wards_2022.csv</t>
+        </is>
+      </c>
+      <c r="I440" t="inlineStr">
+        <is>
+          <t>24_031_701900, 24_031_701701, 24_031_701702, 24_031_701703, 24_031_701704</t>
+        </is>
+      </c>
+      <c r="J440" t="inlineStr">
+        <is>
+          <t>2.9626492758203975e-05, 0.08240206940034545, 0.0001918013454299876, 0.29531273997629875, 0.5644032113171775</t>
+        </is>
+      </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
@@ -20055,11 +20055,19 @@
       </c>
       <c r="H441" t="inlineStr">
         <is>
-          <t>san_francisco_city_council_2022.csv</t>
-        </is>
-      </c>
-      <c r="I441" t="inlineStr"/>
-      <c r="J441" t="inlineStr"/>
+          <t>takoma_park_wards_2022.csv</t>
+        </is>
+      </c>
+      <c r="I441" t="inlineStr">
+        <is>
+          <t>24_031_701701, 24_031_701800, 24_031_702401</t>
+        </is>
+      </c>
+      <c r="J441" t="inlineStr">
+        <is>
+          <t>0.03667248942826369, 0.2692150429403143, 0.0030299499031383142</t>
+        </is>
+      </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">

</xml_diff>